<commit_message>
commit modify review controller
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\food-truck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projectd\food-truck\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>프로젝트 일정 계획표</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -268,15 +268,27 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>축제게시판, 등록, 수정, 고객센터, 등록, 수정, 메인페이지</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">트럭리스트, 트럭검색, 푸드리스트(사용자, 사업자), 트럭지도, </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>역할분담</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>박대현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>박대현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>축제게시판, 고객센터 : 등록, 수정, 삭제, 리스트, 상세보기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객센터 : 등록, 수정, 삭제, 리스트, 상세보기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -372,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="80">
+  <borders count="81">
     <border>
       <left/>
       <right/>
@@ -1419,6 +1431,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1428,24 +1453,372 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1459,361 +1832,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3367,7 +3398,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3663,10 +3694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5325882-A45D-4532-BD89-0B700B7A9056}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3678,947 +3709,926 @@
     <col min="5" max="14" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
     </row>
-    <row r="2" spans="1:14" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="116" t="s">
+    <row r="2" spans="1:22" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="114"/>
+      <c r="D4" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="F4" s="123"/>
+      <c r="G4" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="125"/>
+      <c r="P4" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13" t="s">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="86"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13" t="s">
+      <c r="H5" s="106"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="14"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="126"/>
+      <c r="P5" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q5" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="79"/>
+      <c r="U5" s="79"/>
+      <c r="V5" s="80"/>
     </row>
-    <row r="6" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="91" t="s">
+    <row r="6" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="87"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="92" t="s">
+      <c r="F6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="93" t="s">
+      <c r="H6" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="92" t="s">
+      <c r="I6" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="93" t="s">
+      <c r="J6" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="93" t="s">
+      <c r="K6" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="93" t="s">
+      <c r="L6" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="93" t="s">
+      <c r="M6" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="94" t="s">
+      <c r="N6" s="59" t="s">
         <v>37</v>
       </c>
+      <c r="P6" s="77" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="82"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="7"/>
+      <c r="P7" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" s="127" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="110"/>
+      <c r="S7" s="110"/>
+      <c r="T7" s="110"/>
+      <c r="U7" s="110"/>
+      <c r="V7" s="128"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="98" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="86"/>
+      <c r="B8" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="112"/>
+      <c r="D8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="32"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
+      <c r="P8" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="82"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="87" t="s">
+    <row r="9" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="86"/>
+      <c r="B9" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34" t="s">
+      <c r="C9" s="94"/>
+      <c r="D9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="32"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="13"/>
+      <c r="P9" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="83" t="s">
+        <v>62</v>
+      </c>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="83"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="84"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="87" t="s">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="86"/>
+      <c r="B10" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34" t="s">
+      <c r="C10" s="94"/>
+      <c r="D10" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="32"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="87" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="86"/>
+      <c r="B11" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34" t="s">
+      <c r="C11" s="94"/>
+      <c r="D11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="32"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="86" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="86"/>
+      <c r="B12" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="32"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="13"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="99" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="86"/>
+      <c r="B13" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="32"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="37" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="86"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="32"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="87" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="86"/>
+      <c r="B15" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="94"/>
+      <c r="D15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="32"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="87" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="86"/>
+      <c r="B16" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34" t="s">
+      <c r="C16" s="94"/>
+      <c r="D16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="32"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="13"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="87" t="s">
+      <c r="A17" s="86"/>
+      <c r="B17" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34" t="s">
+      <c r="C17" s="94"/>
+      <c r="D17" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="32"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="87" t="s">
+      <c r="A18" s="86"/>
+      <c r="B18" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34" t="s">
+      <c r="C18" s="94"/>
+      <c r="D18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="32"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="13"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="87" t="s">
+      <c r="A19" s="86"/>
+      <c r="B19" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34" t="s">
+      <c r="C19" s="94"/>
+      <c r="D19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="32"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="13"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="100" t="s">
+      <c r="A20" s="86"/>
+      <c r="B20" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="32"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="13"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="100"/>
-      <c r="C21" s="40" t="s">
+      <c r="A21" s="86"/>
+      <c r="B21" s="121"/>
+      <c r="C21" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="32"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="100"/>
-      <c r="C22" s="37" t="s">
+      <c r="A22" s="86"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="32"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="87" t="s">
+      <c r="A23" s="86"/>
+      <c r="B23" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34" t="s">
+      <c r="C23" s="94"/>
+      <c r="D23" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="32"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="87" t="s">
+      <c r="A24" s="86"/>
+      <c r="B24" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="43" t="s">
+      <c r="C24" s="94"/>
+      <c r="D24" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="44"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="47"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
+      <c r="M24" s="24"/>
+      <c r="N24" s="25"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="88" t="s">
+      <c r="A25" s="86"/>
+      <c r="B25" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="73"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="44"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="87" t="s">
+      <c r="A26" s="86"/>
+      <c r="B26" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="34" t="s">
+      <c r="C26" s="94"/>
+      <c r="D26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="32"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="99" t="s">
+      <c r="A27" s="86"/>
+      <c r="B27" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="32"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="13"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="37" t="s">
+      <c r="A28" s="86"/>
+      <c r="B28" s="110"/>
+      <c r="C28" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="47"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="25"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="88" t="s">
+      <c r="A29" s="86"/>
+      <c r="B29" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="83"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="72"/>
-      <c r="M29" s="72"/>
-      <c r="N29" s="73"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="44"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="87" t="s">
+      <c r="A30" s="86"/>
+      <c r="B30" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="34" t="s">
+      <c r="C30" s="94"/>
+      <c r="D30" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="32"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="13"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="87" t="s">
+      <c r="A31" s="86"/>
+      <c r="B31" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="32"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="13"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="87" t="s">
+      <c r="A32" s="86"/>
+      <c r="B32" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="32"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
-      <c r="B33" s="87" t="s">
+      <c r="A33" s="86"/>
+      <c r="B33" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="47"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="25"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="101" t="s">
+      <c r="A34" s="86"/>
+      <c r="B34" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="102"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="104"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="103"/>
-      <c r="K34" s="105"/>
-      <c r="L34" s="106"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="108"/>
+      <c r="C34" s="96"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="67"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
-      <c r="B35" s="84" t="s">
+      <c r="A35" s="103"/>
+      <c r="B35" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="85"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="109"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="111"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="90"/>
-      <c r="M35" s="90"/>
-      <c r="N35" s="96"/>
+      <c r="C35" s="101"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="61"/>
     </row>
     <row r="36" spans="1:14" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="48"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="50"/>
+      <c r="A36" s="97"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="98"/>
+      <c r="K36" s="98"/>
+      <c r="L36" s="98"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="99"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="85"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="56"/>
+      <c r="C37" s="101"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="30"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="38" t="s">
+      <c r="A38" s="86"/>
+      <c r="B38" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="57"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="31"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="31"/>
-      <c r="N38" s="32"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="13"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="31"/>
-      <c r="L39" s="31"/>
-      <c r="M39" s="31"/>
-      <c r="N39" s="32"/>
+      <c r="A39" s="86"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="12"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="13"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="38" t="s">
+      <c r="A40" s="86"/>
+      <c r="B40" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="47"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="50"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="25"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="84" t="s">
+      <c r="A41" s="86"/>
+      <c r="B41" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="85"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="72"/>
-      <c r="M41" s="72"/>
-      <c r="N41" s="73"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="44"/>
     </row>
     <row r="42" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="15"/>
-      <c r="B42" s="61" t="s">
+      <c r="A42" s="87"/>
+      <c r="B42" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="62"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="66"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="64"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="67"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="38"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="112"/>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114"/>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-    </row>
-    <row r="44" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="117" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" s="115"/>
-      <c r="C44" s="115"/>
-      <c r="D44" s="115"/>
-      <c r="E44" s="115"/>
-      <c r="F44" s="115"/>
-      <c r="G44" s="115"/>
-      <c r="H44" s="115"/>
-      <c r="I44" s="115"/>
-      <c r="J44" s="115"/>
-      <c r="K44" s="115"/>
-      <c r="L44" s="115"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="118" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="119" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="119"/>
-      <c r="D45" s="119"/>
-      <c r="E45" s="119"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="119"/>
-      <c r="K45" s="119"/>
-      <c r="L45" s="119"/>
-      <c r="M45" s="119"/>
-      <c r="N45" s="120"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" s="121" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="122" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="122"/>
-      <c r="D46" s="122"/>
-      <c r="E46" s="122"/>
-      <c r="F46" s="122"/>
-      <c r="G46" s="122"/>
-      <c r="H46" s="122"/>
-      <c r="I46" s="122"/>
-      <c r="J46" s="122"/>
-      <c r="K46" s="122"/>
-      <c r="L46" s="122"/>
-      <c r="M46" s="122"/>
-      <c r="N46" s="123"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" s="121" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="122"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="122"/>
-      <c r="F47" s="122"/>
-      <c r="G47" s="122"/>
-      <c r="H47" s="122"/>
-      <c r="I47" s="122"/>
-      <c r="J47" s="122"/>
-      <c r="K47" s="122"/>
-      <c r="L47" s="122"/>
-      <c r="M47" s="122"/>
-      <c r="N47" s="123"/>
-    </row>
-    <row r="48" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="124" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="125" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="125"/>
-      <c r="D48" s="125"/>
-      <c r="E48" s="125"/>
-      <c r="F48" s="125"/>
-      <c r="G48" s="125"/>
-      <c r="H48" s="125"/>
-      <c r="I48" s="125"/>
-      <c r="J48" s="125"/>
-      <c r="K48" s="125"/>
-      <c r="L48" s="125"/>
-      <c r="M48" s="125"/>
-      <c r="N48" s="126"/>
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="73"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="73"/>
+      <c r="M43" s="73"/>
+      <c r="N43" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B45:N45"/>
-    <mergeCell ref="B46:N46"/>
-    <mergeCell ref="B47:N47"/>
-    <mergeCell ref="B48:N48"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:C42"/>
+  <mergeCells count="47">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:N4"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
@@ -4628,8 +4638,6 @@
     <mergeCell ref="A7:A35"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="D4:D6"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B19:C19"/>
@@ -4637,26 +4645,17 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:N4"/>
-    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="Q5:V5"/>
+    <mergeCell ref="Q6:V6"/>
+    <mergeCell ref="Q8:V8"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="Q7:V7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E8">

</xml_diff>